<commit_message>
Test data sheet for TC-0220
</commit_message>
<xml_diff>
--- a/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
+++ b/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhasip\Desktop\NGConsys Automation_22_03_2019- Purvi\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -255,11 +255,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -289,15 +300,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +714,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L7" sqref="L7:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,12 +735,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -737,10 +749,10 @@
       <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -780,10 +792,10 @@
         <v>38</v>
       </c>
       <c r="N5" s="9">
-        <v>0.32</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="O5" s="9">
-        <v>0.48599999999999999</v>
+        <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -791,10 +803,10 @@
         <v>39</v>
       </c>
       <c r="N6" s="9">
-        <v>0.32</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="O6" s="9">
-        <v>0.48599999999999999</v>
+        <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -831,14 +843,15 @@
       <c r="K7" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="L7" s="16"/>
       <c r="M7" s="8" t="s">
         <v>40</v>
       </c>
       <c r="N7" s="9">
-        <v>0.29799999999999999</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="O7" s="9">
-        <v>0.45600000000000002</v>
+        <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -848,7 +861,7 @@
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -870,10 +883,10 @@
         <v>36</v>
       </c>
       <c r="J8" s="9">
-        <v>0.29799999999999999</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="K8" s="9">
-        <v>0.45600000000000002</v>
+        <v>0.42599999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alarm Normal load method changes
</commit_message>
<xml_diff>
--- a/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
+++ b/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Color Codes</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>MPM800-1</t>
+  </si>
+  <si>
+    <t>AlarmLoadingDetail</t>
+  </si>
+  <si>
+    <t>StandbyLoadingDetail</t>
+  </si>
+  <si>
+    <t>Battery Alarm (A)</t>
+  </si>
+  <si>
+    <t>Battery Standby (A)</t>
   </si>
 </sst>
 </file>
@@ -303,13 +315,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,10 +723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,27 +746,27 @@
     <col min="14" max="15" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -764,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -783,7 +795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="12"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
@@ -798,7 +810,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M6" s="8" t="s">
         <v>39</v>
       </c>
@@ -809,7 +821,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -843,7 +855,7 @@
       <c r="K7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="16"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="8" t="s">
         <v>40</v>
       </c>
@@ -853,8 +865,14 @@
       <c r="O7" s="9">
         <v>0.42599999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
@@ -887,6 +905,12 @@
       </c>
       <c r="K8" s="9">
         <v>0.42599999999999999</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test data as per new implemenation
</commit_message>
<xml_diff>
--- a/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
+++ b/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\consys-uiauto\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -165,10 +165,10 @@
     <t>StandbyLoadingDetail</t>
   </si>
   <si>
-    <t>Battery Alarm (A)</t>
-  </si>
-  <si>
-    <t>Battery Standby (A)</t>
+    <t>Standby Current(A)</t>
+  </si>
+  <si>
+    <t>Alarm Current(A)</t>
   </si>
 </sst>
 </file>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,6 +744,8 @@
     <col min="12" max="12" width="23.21875" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -907,10 +909,10 @@
         <v>0.42599999999999999</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test data for TC-220
</commit_message>
<xml_diff>
--- a/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
+++ b/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
@@ -726,7 +726,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,10 +909,10 @@
         <v>0.42599999999999999</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test data for normal load, cable capacitance etc
</commit_message>
<xml_diff>
--- a/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
+++ b/Test Data/TC-0220_Verify_The_Respective_Normal_Load_Alarm_Load_Property_On_Changing_Power_Source.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F4AC9-680A-487D-8FFD-F3E53D8493AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,7 +602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -722,11 +723,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,10 +807,10 @@
         <v>38</v>
       </c>
       <c r="N5" s="9">
-        <v>0.28599999999999998</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="O5" s="9">
-        <v>0.44500000000000001</v>
+        <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -817,10 +818,10 @@
         <v>39</v>
       </c>
       <c r="N6" s="9">
-        <v>0.28599999999999998</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="O6" s="9">
-        <v>0.44500000000000001</v>
+        <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>